<commit_message>
EDSF-74: Update Excel inputs, but still have one test failing for somewhat mysterious reasons, need to look deeper
</commit_message>
<xml_diff>
--- a/EduSafe.Core.Tests/Resources/Dropout-Rate-Test-Scenarios-Single.xlsx
+++ b/EduSafe.Core.Tests/Resources/Dropout-Rate-Test-Scenarios-Single.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.Core.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0431F4-FFC0-43B9-BFB4-A1DB0AB2DF6C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF87D6F5-A32D-4289-B66A-777405430574}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="525" windowWidth="15915" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="2" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>Period</t>
   </si>
   <si>
-    <t>Income</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -247,10 +244,13 @@
     <t>Interest Rate Types</t>
   </si>
   <si>
-    <t>CoverageMonths</t>
-  </si>
-  <si>
-    <t>AnnualIncome</t>
+    <t>UnemploymentCoverage</t>
+  </si>
+  <si>
+    <t>DropOutWarranty</t>
+  </si>
+  <si>
+    <t>WarrantyCoverageMonths</t>
   </si>
 </sst>
 </file>
@@ -301,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,12 +317,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +353,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -425,9 +419,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -779,11 +770,11 @@
   <dimension ref="B2:X3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C8" sqref="C8"/>
       <selection pane="topRight" activeCell="C8" sqref="C8"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -804,8 +795,9 @@
     <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="23.140625" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
+    <col min="19" max="19" width="24.42578125" customWidth="1"/>
     <col min="20" max="20" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -814,25 +806,25 @@
   <sheetData>
     <row r="2" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>1</v>
@@ -847,40 +839,40 @@
         <v>4</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="P2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
@@ -897,13 +889,13 @@
       <c r="E3" s="9">
         <v>5</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="28">
         <v>0.25</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="28">
         <v>0.25</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="28">
         <v>0.25</v>
       </c>
       <c r="I3">
@@ -935,18 +927,17 @@
       <c r="Q3" s="10">
         <v>25000</v>
       </c>
-      <c r="R3" s="28">
-        <f>Q3 * (12 / S3)</f>
-        <v>50000</v>
+      <c r="R3" s="10">
+        <v>0</v>
       </c>
       <c r="S3" s="10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U3" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V3" s="10">
         <v>1</v>
@@ -992,21 +983,21 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="7">
         <v>100</v>
@@ -1017,7 +1008,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7">
         <v>25</v>
@@ -1028,7 +1019,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7">
         <v>25</v>
@@ -1039,7 +1030,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7">
         <v>20</v>
@@ -1050,50 +1041,50 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="7">
         <v>150</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="7">
         <v>150</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="7">
         <v>300</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7">
         <v>1000</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1125,53 +1116,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2463,15 +2454,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="26">
         <v>43453</v>
@@ -2482,14 +2473,14 @@
         <v>9</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>0</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2497,7 +2488,7 @@
       <c r="A5" s="20">
         <v>1</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2505,7 +2496,7 @@
       <c r="A6" s="20">
         <v>2</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2513,7 +2504,7 @@
       <c r="A7" s="20">
         <v>3</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2521,7 +2512,7 @@
       <c r="A8" s="20">
         <v>4</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2529,7 +2520,7 @@
       <c r="A9" s="20">
         <v>5</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2537,7 +2528,7 @@
       <c r="A10" s="20">
         <v>6</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2545,7 +2536,7 @@
       <c r="A11" s="20">
         <v>7</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2553,7 +2544,7 @@
       <c r="A12" s="20">
         <v>8</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2561,7 +2552,7 @@
       <c r="A13" s="20">
         <v>9</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2569,7 +2560,7 @@
       <c r="A14" s="20">
         <v>10</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2577,7 +2568,7 @@
       <c r="A15" s="20">
         <v>11</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2585,7 +2576,7 @@
       <c r="A16" s="20">
         <v>12</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2593,7 +2584,7 @@
       <c r="A17" s="20">
         <v>13</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2601,7 +2592,7 @@
       <c r="A18" s="20">
         <v>14</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2609,7 +2600,7 @@
       <c r="A19" s="20">
         <v>15</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2617,7 +2608,7 @@
       <c r="A20" s="20">
         <v>16</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2625,7 +2616,7 @@
       <c r="A21" s="20">
         <v>17</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2633,7 +2624,7 @@
       <c r="A22" s="20">
         <v>18</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2641,7 +2632,7 @@
       <c r="A23" s="20">
         <v>19</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2649,7 +2640,7 @@
       <c r="A24" s="20">
         <v>20</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B24" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2657,7 +2648,7 @@
       <c r="A25" s="20">
         <v>21</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2665,7 +2656,7 @@
       <c r="A26" s="20">
         <v>22</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2673,7 +2664,7 @@
       <c r="A27" s="20">
         <v>23</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2681,7 +2672,7 @@
       <c r="A28" s="20">
         <v>24</v>
       </c>
-      <c r="B28" s="30">
+      <c r="B28" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2689,7 +2680,7 @@
       <c r="A29" s="20">
         <v>25</v>
       </c>
-      <c r="B29" s="30">
+      <c r="B29" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2697,7 +2688,7 @@
       <c r="A30" s="20">
         <v>26</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2705,7 +2696,7 @@
       <c r="A31" s="20">
         <v>27</v>
       </c>
-      <c r="B31" s="30">
+      <c r="B31" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2713,7 +2704,7 @@
       <c r="A32" s="20">
         <v>28</v>
       </c>
-      <c r="B32" s="30">
+      <c r="B32" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2721,7 +2712,7 @@
       <c r="A33" s="20">
         <v>29</v>
       </c>
-      <c r="B33" s="30">
+      <c r="B33" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2729,7 +2720,7 @@
       <c r="A34" s="20">
         <v>30</v>
       </c>
-      <c r="B34" s="30">
+      <c r="B34" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2737,7 +2728,7 @@
       <c r="A35" s="20">
         <v>31</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B35" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2745,7 +2736,7 @@
       <c r="A36" s="20">
         <v>32</v>
       </c>
-      <c r="B36" s="30">
+      <c r="B36" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2753,7 +2744,7 @@
       <c r="A37" s="20">
         <v>33</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B37" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2761,7 +2752,7 @@
       <c r="A38" s="20">
         <v>34</v>
       </c>
-      <c r="B38" s="30">
+      <c r="B38" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2769,7 +2760,7 @@
       <c r="A39" s="20">
         <v>35</v>
       </c>
-      <c r="B39" s="30">
+      <c r="B39" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2777,7 +2768,7 @@
       <c r="A40" s="20">
         <v>36</v>
       </c>
-      <c r="B40" s="30">
+      <c r="B40" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2785,7 +2776,7 @@
       <c r="A41" s="20">
         <v>37</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B41" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2793,7 +2784,7 @@
       <c r="A42" s="20">
         <v>38</v>
       </c>
-      <c r="B42" s="30">
+      <c r="B42" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2801,7 +2792,7 @@
       <c r="A43" s="20">
         <v>39</v>
       </c>
-      <c r="B43" s="30">
+      <c r="B43" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2809,7 +2800,7 @@
       <c r="A44" s="20">
         <v>40</v>
       </c>
-      <c r="B44" s="30">
+      <c r="B44" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2817,7 +2808,7 @@
       <c r="A45" s="20">
         <v>41</v>
       </c>
-      <c r="B45" s="30">
+      <c r="B45" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2825,7 +2816,7 @@
       <c r="A46" s="20">
         <v>42</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2833,7 +2824,7 @@
       <c r="A47" s="20">
         <v>43</v>
       </c>
-      <c r="B47" s="30">
+      <c r="B47" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2841,7 +2832,7 @@
       <c r="A48" s="20">
         <v>44</v>
       </c>
-      <c r="B48" s="30">
+      <c r="B48" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2849,7 +2840,7 @@
       <c r="A49" s="20">
         <v>45</v>
       </c>
-      <c r="B49" s="30">
+      <c r="B49" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2857,7 +2848,7 @@
       <c r="A50" s="20">
         <v>46</v>
       </c>
-      <c r="B50" s="30">
+      <c r="B50" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2865,7 +2856,7 @@
       <c r="A51" s="20">
         <v>47</v>
       </c>
-      <c r="B51" s="30">
+      <c r="B51" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2873,7 +2864,7 @@
       <c r="A52" s="20">
         <v>48</v>
       </c>
-      <c r="B52" s="30">
+      <c r="B52" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2881,7 +2872,7 @@
       <c r="A53" s="20">
         <v>49</v>
       </c>
-      <c r="B53" s="30">
+      <c r="B53" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2889,7 +2880,7 @@
       <c r="A54" s="20">
         <v>50</v>
       </c>
-      <c r="B54" s="30">
+      <c r="B54" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2897,7 +2888,7 @@
       <c r="A55" s="20">
         <v>51</v>
       </c>
-      <c r="B55" s="30">
+      <c r="B55" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2905,7 +2896,7 @@
       <c r="A56" s="20">
         <v>52</v>
       </c>
-      <c r="B56" s="30">
+      <c r="B56" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2913,7 +2904,7 @@
       <c r="A57" s="20">
         <v>53</v>
       </c>
-      <c r="B57" s="30">
+      <c r="B57" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2921,7 +2912,7 @@
       <c r="A58" s="20">
         <v>54</v>
       </c>
-      <c r="B58" s="30">
+      <c r="B58" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2929,7 +2920,7 @@
       <c r="A59" s="20">
         <v>55</v>
       </c>
-      <c r="B59" s="30">
+      <c r="B59" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2937,7 +2928,7 @@
       <c r="A60" s="20">
         <v>56</v>
       </c>
-      <c r="B60" s="30">
+      <c r="B60" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2945,7 +2936,7 @@
       <c r="A61" s="20">
         <v>57</v>
       </c>
-      <c r="B61" s="30">
+      <c r="B61" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2953,7 +2944,7 @@
       <c r="A62" s="20">
         <v>58</v>
       </c>
-      <c r="B62" s="30">
+      <c r="B62" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2961,7 +2952,7 @@
       <c r="A63" s="20">
         <v>59</v>
       </c>
-      <c r="B63" s="30">
+      <c r="B63" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2969,7 +2960,7 @@
       <c r="A64" s="20">
         <v>60</v>
       </c>
-      <c r="B64" s="30">
+      <c r="B64" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2977,7 +2968,7 @@
       <c r="A65" s="20">
         <v>61</v>
       </c>
-      <c r="B65" s="30">
+      <c r="B65" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2985,7 +2976,7 @@
       <c r="A66" s="20">
         <v>62</v>
       </c>
-      <c r="B66" s="30">
+      <c r="B66" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -2993,7 +2984,7 @@
       <c r="A67" s="20">
         <v>63</v>
       </c>
-      <c r="B67" s="30">
+      <c r="B67" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3001,7 +2992,7 @@
       <c r="A68" s="20">
         <v>64</v>
       </c>
-      <c r="B68" s="30">
+      <c r="B68" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3009,7 +3000,7 @@
       <c r="A69" s="20">
         <v>65</v>
       </c>
-      <c r="B69" s="30">
+      <c r="B69" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3017,7 +3008,7 @@
       <c r="A70" s="20">
         <v>66</v>
       </c>
-      <c r="B70" s="30">
+      <c r="B70" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3025,7 +3016,7 @@
       <c r="A71" s="20">
         <v>67</v>
       </c>
-      <c r="B71" s="30">
+      <c r="B71" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3033,7 +3024,7 @@
       <c r="A72" s="20">
         <v>68</v>
       </c>
-      <c r="B72" s="30">
+      <c r="B72" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3041,7 +3032,7 @@
       <c r="A73" s="20">
         <v>69</v>
       </c>
-      <c r="B73" s="30">
+      <c r="B73" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3049,7 +3040,7 @@
       <c r="A74" s="20">
         <v>70</v>
       </c>
-      <c r="B74" s="30">
+      <c r="B74" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3057,7 +3048,7 @@
       <c r="A75" s="20">
         <v>71</v>
       </c>
-      <c r="B75" s="30">
+      <c r="B75" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3065,7 +3056,7 @@
       <c r="A76" s="21">
         <v>72</v>
       </c>
-      <c r="B76" s="30">
+      <c r="B76" s="29">
         <v>2.35E-2</v>
       </c>
     </row>
@@ -3091,125 +3082,125 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="27"/>
       <c r="C5" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="27"/>
       <c r="C6" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="27"/>
       <c r="C7" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="D9" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="D10" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
       <c r="D11" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
       <c r="D12" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
       <c r="D13" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
       <c r="D16" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>